<commit_message>
Cambio IPNC en nomina y hospedaje
</commit_message>
<xml_diff>
--- a/Calculos_2015.xlsx
+++ b/Calculos_2015.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dtax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dtax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D243794-C7CD-47AD-8F19-9675DCFFE83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E043EB4E-05EE-4334-BF41-4D716C5E961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="717" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="717" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAL_ISR_2012" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,17 @@
     <sheet name="IVA Arrendamiento" sheetId="4" r:id="rId5"/>
     <sheet name="IVA RIF" sheetId="5" r:id="rId6"/>
     <sheet name="Hoja1" sheetId="6" r:id="rId7"/>
+    <sheet name="Imp hospedaje 22" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -513,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="670">
   <si>
     <t>clave</t>
   </si>
@@ -2486,18 +2490,79 @@
   <si>
     <t>V52</t>
   </si>
+  <si>
+    <t xml:space="preserve">Total de base Gravable                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasa de Impuesto sobre Nomina                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impuesto sobre Nomina                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualización                                               </t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>N7</t>
+  </si>
+  <si>
+    <t>N8</t>
+  </si>
+  <si>
+    <t>N9</t>
+  </si>
+  <si>
+    <t>N10</t>
+  </si>
+  <si>
+    <t>N11</t>
+  </si>
+  <si>
+    <t>N12</t>
+  </si>
+  <si>
+    <t>INPC Anterior al Ultimo Conocido (sep-22)</t>
+  </si>
+  <si>
+    <t>INPC Anterior que Debio Pagarse (ene-22)</t>
+  </si>
+  <si>
+    <t>Impto actualizado</t>
+  </si>
+  <si>
+    <t>(-) impuesto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2753,8 +2818,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2884,6 +2962,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3266,7 +3350,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3742,55 +3826,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3853,6 +3889,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="35" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="35" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="35" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="35" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="36" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Énfasis5" xfId="2" builtinId="47"/>
@@ -4270,134 +4375,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A2" s="219" t="s">
+      <c r="A2" s="252" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
-      <c r="I2" s="219"/>
-      <c r="L2" s="220" t="s">
+      <c r="B2" s="252"/>
+      <c r="C2" s="252"/>
+      <c r="D2" s="252"/>
+      <c r="E2" s="252"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="252"/>
+      <c r="H2" s="252"/>
+      <c r="I2" s="252"/>
+      <c r="L2" s="253" t="s">
         <v>350</v>
       </c>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
-      <c r="Q2" s="220"/>
-      <c r="R2" s="220"/>
-      <c r="S2" s="220"/>
-      <c r="T2" s="220"/>
-      <c r="W2" s="221" t="s">
+      <c r="M2" s="253"/>
+      <c r="N2" s="253"/>
+      <c r="O2" s="253"/>
+      <c r="P2" s="253"/>
+      <c r="Q2" s="253"/>
+      <c r="R2" s="253"/>
+      <c r="S2" s="253"/>
+      <c r="T2" s="253"/>
+      <c r="W2" s="254" t="s">
         <v>350</v>
       </c>
-      <c r="X2" s="221"/>
-      <c r="Y2" s="221"/>
-      <c r="Z2" s="221"/>
-      <c r="AA2" s="221"/>
-      <c r="AB2" s="221"/>
-      <c r="AC2" s="221"/>
-      <c r="AD2" s="221"/>
-      <c r="AE2" s="221"/>
-      <c r="AF2" s="221"/>
-      <c r="AK2" s="213" t="s">
+      <c r="X2" s="254"/>
+      <c r="Y2" s="254"/>
+      <c r="Z2" s="254"/>
+      <c r="AA2" s="254"/>
+      <c r="AB2" s="254"/>
+      <c r="AC2" s="254"/>
+      <c r="AD2" s="254"/>
+      <c r="AE2" s="254"/>
+      <c r="AF2" s="254"/>
+      <c r="AK2" s="246" t="s">
         <v>350</v>
       </c>
-      <c r="AL2" s="213"/>
-      <c r="AM2" s="213"/>
-      <c r="AN2" s="213"/>
-      <c r="AO2" s="213"/>
-      <c r="AP2" s="213"/>
-      <c r="AQ2" s="213"/>
-      <c r="AR2" s="213"/>
-      <c r="AS2" s="213"/>
-      <c r="AX2" s="213" t="s">
+      <c r="AL2" s="246"/>
+      <c r="AM2" s="246"/>
+      <c r="AN2" s="246"/>
+      <c r="AO2" s="246"/>
+      <c r="AP2" s="246"/>
+      <c r="AQ2" s="246"/>
+      <c r="AR2" s="246"/>
+      <c r="AS2" s="246"/>
+      <c r="AX2" s="246" t="s">
         <v>350</v>
       </c>
-      <c r="AY2" s="213"/>
-      <c r="AZ2" s="213"/>
-      <c r="BA2" s="213"/>
-      <c r="BB2" s="213"/>
-      <c r="BC2" s="213"/>
-      <c r="BD2" s="213"/>
-      <c r="BE2" s="213"/>
-      <c r="BF2" s="213"/>
+      <c r="AY2" s="246"/>
+      <c r="AZ2" s="246"/>
+      <c r="BA2" s="246"/>
+      <c r="BB2" s="246"/>
+      <c r="BC2" s="246"/>
+      <c r="BD2" s="246"/>
+      <c r="BE2" s="246"/>
+      <c r="BF2" s="246"/>
       <c r="BG2" s="198"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="257" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="222" t="s">
+      <c r="B4" s="257"/>
+      <c r="C4" s="255" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="217"/>
-      <c r="G4" s="217"/>
-      <c r="H4" s="217"/>
-      <c r="I4" s="218"/>
+      <c r="D4" s="250"/>
+      <c r="E4" s="250"/>
+      <c r="F4" s="250"/>
+      <c r="G4" s="250"/>
+      <c r="H4" s="250"/>
+      <c r="I4" s="251"/>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
-      <c r="L4" s="227" t="s">
+      <c r="L4" s="260" t="s">
         <v>227</v>
       </c>
-      <c r="M4" s="228"/>
+      <c r="M4" s="261"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="222" t="s">
+      <c r="O4" s="255" t="s">
         <v>285</v>
       </c>
-      <c r="P4" s="217"/>
-      <c r="Q4" s="217"/>
-      <c r="R4" s="217"/>
-      <c r="S4" s="218"/>
+      <c r="P4" s="250"/>
+      <c r="Q4" s="250"/>
+      <c r="R4" s="250"/>
+      <c r="S4" s="251"/>
       <c r="T4" s="36"/>
       <c r="U4" s="36"/>
-      <c r="W4" s="225" t="s">
+      <c r="W4" s="258" t="s">
         <v>227</v>
       </c>
-      <c r="X4" s="225"/>
+      <c r="X4" s="258"/>
       <c r="Y4" s="68"/>
-      <c r="Z4" s="226" t="s">
+      <c r="Z4" s="259" t="s">
         <v>288</v>
       </c>
-      <c r="AA4" s="226"/>
-      <c r="AB4" s="226"/>
-      <c r="AC4" s="226"/>
-      <c r="AD4" s="226"/>
-      <c r="AE4" s="226"/>
-      <c r="AF4" s="226"/>
-      <c r="AK4" s="214" t="s">
+      <c r="AA4" s="259"/>
+      <c r="AB4" s="259"/>
+      <c r="AC4" s="259"/>
+      <c r="AD4" s="259"/>
+      <c r="AE4" s="259"/>
+      <c r="AF4" s="259"/>
+      <c r="AK4" s="247" t="s">
         <v>227</v>
       </c>
-      <c r="AL4" s="215"/>
+      <c r="AL4" s="248"/>
       <c r="AM4" s="78"/>
-      <c r="AN4" s="222" t="s">
+      <c r="AN4" s="255" t="s">
         <v>364</v>
       </c>
-      <c r="AO4" s="217"/>
-      <c r="AP4" s="217"/>
-      <c r="AQ4" s="217"/>
-      <c r="AR4" s="218"/>
+      <c r="AO4" s="250"/>
+      <c r="AP4" s="250"/>
+      <c r="AQ4" s="250"/>
+      <c r="AR4" s="251"/>
       <c r="AS4" s="78"/>
       <c r="AT4" s="78"/>
-      <c r="AX4" s="214" t="s">
+      <c r="AX4" s="247" t="s">
         <v>227</v>
       </c>
-      <c r="AY4" s="215"/>
+      <c r="AY4" s="248"/>
       <c r="AZ4" s="171"/>
-      <c r="BA4" s="216" t="s">
+      <c r="BA4" s="249" t="s">
         <v>561</v>
       </c>
-      <c r="BB4" s="217"/>
-      <c r="BC4" s="217"/>
-      <c r="BD4" s="217"/>
-      <c r="BE4" s="218"/>
+      <c r="BB4" s="250"/>
+      <c r="BC4" s="250"/>
+      <c r="BD4" s="250"/>
+      <c r="BE4" s="251"/>
       <c r="BF4" s="171"/>
       <c r="BG4" s="198"/>
       <c r="BJ4" t="s">
@@ -4818,10 +4923,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="223" t="s">
+      <c r="E8" s="256" t="s">
         <v>308</v>
       </c>
-      <c r="F8" s="223"/>
+      <c r="F8" s="256"/>
       <c r="G8" s="14"/>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -9350,10 +9455,10 @@
       <c r="D52" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E52" s="223" t="s">
+      <c r="E52" s="256" t="s">
         <v>326</v>
       </c>
-      <c r="F52" s="223"/>
+      <c r="F52" s="256"/>
       <c r="G52" s="14"/>
       <c r="H52" s="5" t="s">
         <v>65</v>
@@ -9680,10 +9785,10 @@
       <c r="D56" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E56" s="223" t="s">
+      <c r="E56" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="F56" s="223"/>
+      <c r="F56" s="256"/>
       <c r="G56" s="14"/>
       <c r="H56" s="5" t="s">
         <v>72</v>
@@ -10066,16 +10171,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="262" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="229"/>
+      <c r="B1" s="262"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
-      <c r="G1" s="229" t="s">
+      <c r="G1" s="262" t="s">
         <v>228</v>
       </c>
-      <c r="H1" s="229"/>
+      <c r="H1" s="262"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -13013,8 +13118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5823B452-03D9-4047-8871-7B00A250D938}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13102,12 +13207,12 @@
       <c r="E3" s="104" t="s">
         <v>645</v>
       </c>
-      <c r="F3" s="249"/>
-      <c r="G3" s="250"/>
-      <c r="H3" s="251" t="s">
+      <c r="F3" s="233"/>
+      <c r="G3" s="234"/>
+      <c r="H3" s="235" t="s">
         <v>617</v>
       </c>
-      <c r="I3" s="252" t="s">
+      <c r="I3" s="236" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13243,10 +13348,10 @@
       <c r="B9" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="230" t="s">
+      <c r="C9" s="214" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="231" t="s">
+      <c r="D9" s="215" t="s">
         <v>199</v>
       </c>
       <c r="E9" s="104"/>
@@ -13266,10 +13371,10 @@
       <c r="B10" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="232" t="s">
+      <c r="C10" s="216" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="233" t="s">
+      <c r="D10" s="217" t="s">
         <v>201</v>
       </c>
       <c r="E10" s="104"/>
@@ -13306,10 +13411,10 @@
       <c r="B12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="230" t="s">
+      <c r="C12" s="214" t="s">
         <v>201</v>
       </c>
-      <c r="D12" s="231" t="s">
+      <c r="D12" s="215" t="s">
         <v>205</v>
       </c>
       <c r="E12" s="104"/>
@@ -13329,10 +13434,10 @@
       <c r="B13" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="C13" s="232" t="s">
+      <c r="C13" s="216" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="233" t="s">
+      <c r="D13" s="217" t="s">
         <v>207</v>
       </c>
       <c r="E13" s="104"/>
@@ -13352,10 +13457,10 @@
       <c r="B14" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="C14" s="234" t="s">
+      <c r="C14" s="218" t="s">
         <v>205</v>
       </c>
-      <c r="D14" s="235" t="s">
+      <c r="D14" s="219" t="s">
         <v>209</v>
       </c>
       <c r="E14" s="104"/>
@@ -13375,10 +13480,10 @@
       <c r="B15" s="72" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="236" t="s">
+      <c r="C15" s="220" t="s">
         <v>207</v>
       </c>
-      <c r="D15" s="237" t="s">
+      <c r="D15" s="221" t="s">
         <v>211</v>
       </c>
       <c r="E15" s="104"/>
@@ -13398,15 +13503,15 @@
       <c r="D16" s="211" t="s">
         <v>213</v>
       </c>
-      <c r="E16" s="253" t="s">
+      <c r="E16" s="237" t="s">
         <v>646</v>
       </c>
-      <c r="F16" s="254"/>
-      <c r="G16" s="255"/>
-      <c r="H16" s="256" t="s">
+      <c r="F16" s="238"/>
+      <c r="G16" s="239"/>
+      <c r="H16" s="240" t="s">
         <v>619</v>
       </c>
-      <c r="I16" s="257" t="s">
+      <c r="I16" s="241" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13417,15 +13522,15 @@
       <c r="D17" s="211" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="253" t="s">
+      <c r="E17" s="237" t="s">
         <v>647</v>
       </c>
-      <c r="F17" s="254"/>
-      <c r="G17" s="255"/>
-      <c r="H17" s="256" t="s">
+      <c r="F17" s="238"/>
+      <c r="G17" s="239"/>
+      <c r="H17" s="240" t="s">
         <v>620</v>
       </c>
-      <c r="I17" s="257" t="s">
+      <c r="I17" s="241" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13442,17 +13547,17 @@
       <c r="D18" s="120" t="s">
         <v>216</v>
       </c>
-      <c r="E18" s="242"/>
-      <c r="F18" s="243" t="s">
+      <c r="E18" s="226"/>
+      <c r="F18" s="227" t="s">
         <v>626</v>
       </c>
-      <c r="G18" s="244">
+      <c r="G18" s="228">
         <v>9.99</v>
       </c>
-      <c r="H18" s="245" t="s">
+      <c r="H18" s="229" t="s">
         <v>273</v>
       </c>
-      <c r="I18" s="246"/>
+      <c r="I18" s="230"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
@@ -13491,23 +13596,23 @@
       <c r="B20" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="230" t="s">
+      <c r="C20" s="214" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="231" t="s">
+      <c r="D20" s="215" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="238"/>
-      <c r="F20" s="239" t="s">
+      <c r="E20" s="222"/>
+      <c r="F20" s="223" t="s">
         <v>627</v>
       </c>
-      <c r="G20" s="244">
+      <c r="G20" s="228">
         <v>9.99</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="I20" s="240"/>
+      <c r="I20" s="224"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
@@ -13533,23 +13638,23 @@
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="72"/>
       <c r="B22" s="72"/>
-      <c r="C22" s="232" t="s">
+      <c r="C22" s="216" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="233" t="s">
+      <c r="D22" s="217" t="s">
         <v>222</v>
       </c>
-      <c r="E22" s="238"/>
-      <c r="F22" s="239" t="s">
+      <c r="E22" s="222"/>
+      <c r="F22" s="223" t="s">
         <v>628</v>
       </c>
-      <c r="G22" s="244">
+      <c r="G22" s="228">
         <v>9.99</v>
       </c>
       <c r="H22" s="28" t="s">
         <v>387</v>
       </c>
-      <c r="I22" s="240"/>
+      <c r="I22" s="224"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="72"/>
@@ -13575,23 +13680,23 @@
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="72"/>
       <c r="B24" s="72"/>
-      <c r="C24" s="234" t="s">
+      <c r="C24" s="218" t="s">
         <v>219</v>
       </c>
-      <c r="D24" s="235" t="s">
+      <c r="D24" s="219" t="s">
         <v>224</v>
       </c>
-      <c r="E24" s="238"/>
-      <c r="F24" s="239" t="s">
+      <c r="E24" s="222"/>
+      <c r="F24" s="223" t="s">
         <v>629</v>
       </c>
-      <c r="G24" s="244">
+      <c r="G24" s="228">
         <v>9.99</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>389</v>
       </c>
-      <c r="I24" s="240"/>
+      <c r="I24" s="224"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="72"/>
@@ -13617,23 +13722,23 @@
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="72"/>
       <c r="B26" s="72"/>
-      <c r="C26" s="236" t="s">
+      <c r="C26" s="220" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="237" t="s">
+      <c r="D26" s="221" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="238"/>
-      <c r="F26" s="239" t="s">
+      <c r="E26" s="222"/>
+      <c r="F26" s="223" t="s">
         <v>630</v>
       </c>
-      <c r="G26" s="244">
+      <c r="G26" s="228">
         <v>9.99</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>391</v>
       </c>
-      <c r="I26" s="240"/>
+      <c r="I26" s="224"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="72"/>
@@ -13665,17 +13770,17 @@
       <c r="D28" s="120" t="s">
         <v>399</v>
       </c>
-      <c r="E28" s="238"/>
-      <c r="F28" s="239" t="s">
+      <c r="E28" s="222"/>
+      <c r="F28" s="223" t="s">
         <v>631</v>
       </c>
-      <c r="G28" s="244">
+      <c r="G28" s="228">
         <v>9.99</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>393</v>
       </c>
-      <c r="I28" s="240"/>
+      <c r="I28" s="224"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="72"/>
@@ -13707,17 +13812,17 @@
       <c r="D30" s="120" t="s">
         <v>403</v>
       </c>
-      <c r="E30" s="242"/>
-      <c r="F30" s="239" t="s">
+      <c r="E30" s="226"/>
+      <c r="F30" s="223" t="s">
         <v>632</v>
       </c>
-      <c r="G30" s="244">
+      <c r="G30" s="228">
         <v>9.99</v>
       </c>
-      <c r="H30" s="245" t="s">
+      <c r="H30" s="229" t="s">
         <v>395</v>
       </c>
-      <c r="I30" s="246"/>
+      <c r="I30" s="230"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
@@ -13758,17 +13863,17 @@
       <c r="D32" s="120" t="s">
         <v>407</v>
       </c>
-      <c r="E32" s="238"/>
-      <c r="F32" s="239" t="s">
+      <c r="E32" s="222"/>
+      <c r="F32" s="223" t="s">
         <v>633</v>
       </c>
-      <c r="G32" s="244">
+      <c r="G32" s="228">
         <v>9.99</v>
       </c>
       <c r="H32" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="I32" s="240"/>
+      <c r="I32" s="224"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="72"/>
@@ -13781,17 +13886,17 @@
       <c r="D33" s="120" t="s">
         <v>408</v>
       </c>
-      <c r="E33" s="238"/>
-      <c r="F33" s="239" t="s">
+      <c r="E33" s="222"/>
+      <c r="F33" s="223" t="s">
         <v>634</v>
       </c>
-      <c r="G33" s="244">
+      <c r="G33" s="228">
         <v>9.99</v>
       </c>
       <c r="H33" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="I33" s="240"/>
+      <c r="I33" s="224"/>
       <c r="N33" s="203" t="s">
         <v>526</v>
       </c>
@@ -13813,17 +13918,17 @@
       <c r="D34" s="120" t="s">
         <v>409</v>
       </c>
-      <c r="E34" s="238"/>
-      <c r="F34" s="239" t="s">
+      <c r="E34" s="222"/>
+      <c r="F34" s="223" t="s">
         <v>635</v>
       </c>
-      <c r="G34" s="241">
+      <c r="G34" s="225">
         <v>9.99</v>
       </c>
       <c r="H34" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="I34" s="240"/>
+      <c r="I34" s="224"/>
       <c r="J34" s="124" t="s">
         <v>403</v>
       </c>
@@ -13928,17 +14033,17 @@
       <c r="D37" s="120" t="s">
         <v>413</v>
       </c>
-      <c r="E37" s="238"/>
-      <c r="F37" s="247" t="s">
+      <c r="E37" s="222"/>
+      <c r="F37" s="231" t="s">
         <v>636</v>
       </c>
-      <c r="G37" s="244">
+      <c r="G37" s="228">
         <v>9.99</v>
       </c>
       <c r="H37" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="I37" s="240"/>
+      <c r="I37" s="224"/>
       <c r="J37" s="124" t="s">
         <v>408</v>
       </c>
@@ -13969,17 +14074,17 @@
       <c r="D38" s="120" t="s">
         <v>414</v>
       </c>
-      <c r="E38" s="238"/>
-      <c r="F38" s="248" t="s">
+      <c r="E38" s="222"/>
+      <c r="F38" s="232" t="s">
         <v>637</v>
       </c>
-      <c r="G38" s="241">
+      <c r="G38" s="225">
         <v>9.99</v>
       </c>
       <c r="H38" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="I38" s="240"/>
+      <c r="I38" s="224"/>
       <c r="J38" s="124" t="s">
         <v>409</v>
       </c>
@@ -14625,8 +14730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15212,8 +15317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15889,7 +15994,7 @@
   <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16031,4 +16136,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D6352A-C30E-4FA2-BEF1-5CC43B7B90A8}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="243">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="213" t="s">
+        <v>654</v>
+      </c>
+      <c r="B2" s="263">
+        <v>16074</v>
+      </c>
+      <c r="C2" s="242" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="213" t="s">
+        <v>655</v>
+      </c>
+      <c r="B3" s="264">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="213" t="s">
+        <v>656</v>
+      </c>
+      <c r="B4" s="272">
+        <f>+B2*B3</f>
+        <v>401.85</v>
+      </c>
+      <c r="C4" s="242" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="213" t="s">
+        <v>657</v>
+      </c>
+      <c r="B5" s="265">
+        <v>124.571</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="213" t="s">
+        <v>658</v>
+      </c>
+      <c r="B6" s="265">
+        <v>118.002</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="213" t="s">
+        <v>659</v>
+      </c>
+      <c r="B7" s="266">
+        <f>+B5/B6</f>
+        <v>1.055668547990712</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="213" t="s">
+        <v>660</v>
+      </c>
+      <c r="B8" s="274">
+        <f>+B4*B7</f>
+        <v>424.22040601006762</v>
+      </c>
+      <c r="C8" s="242" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="213"/>
+      <c r="B9" s="267">
+        <f>+B4</f>
+        <v>401.85</v>
+      </c>
+      <c r="C9" s="242" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="213"/>
+      <c r="B10" s="267">
+        <f>+B8-B9</f>
+        <v>22.370406010067597</v>
+      </c>
+      <c r="C10" s="242" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="213" t="s">
+        <v>661</v>
+      </c>
+      <c r="B11" s="268">
+        <v>1.47E-2</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="213" t="s">
+        <v>662</v>
+      </c>
+      <c r="B12" s="269">
+        <v>9</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="213" t="s">
+        <v>663</v>
+      </c>
+      <c r="B13" s="270">
+        <f>+B12*B11</f>
+        <v>0.1323</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="213" t="s">
+        <v>664</v>
+      </c>
+      <c r="B14" s="273">
+        <f>+B4*B13</f>
+        <v>53.164755000000007</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="213" t="s">
+        <v>665</v>
+      </c>
+      <c r="B15" s="271">
+        <f>+B4+B10+B14</f>
+        <v>477.38516101006763</v>
+      </c>
+      <c r="C15" s="242" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="244">
+        <f>+B4</f>
+        <v>401.85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="245">
+        <f>+B10</f>
+        <v>22.370406010067597</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="186">
+        <f>+B14</f>
+        <v>53.164755000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="186">
+        <f>+B17+B18+B19</f>
+        <v>477.38516101006763</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion Concentrado sparacion Ret Salarios y Asimilados
</commit_message>
<xml_diff>
--- a/Calculos_2015.xlsx
+++ b/Calculos_2015.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dtax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E043EB4E-05EE-4334-BF41-4D716C5E961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D097970B-ADE3-48D5-8FAC-A41BDBD1A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="717" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="717" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAL_ISR_2012" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="682">
   <si>
     <t>clave</t>
   </si>
@@ -2272,24 +2272,6 @@
   </si>
   <si>
     <t>Compras y Gastos Pagados con Tasa 16%</t>
-  </si>
-  <si>
-    <t>ene</t>
-  </si>
-  <si>
-    <t>feb</t>
-  </si>
-  <si>
-    <t>mar</t>
-  </si>
-  <si>
-    <t>abr</t>
-  </si>
-  <si>
-    <t>1er bim</t>
-  </si>
-  <si>
-    <t>2do bim</t>
   </si>
   <si>
     <t>Si(mes=ene,K9,V16 mes ant)</t>
@@ -2549,6 +2531,60 @@
   </si>
   <si>
     <t>(-) impuesto</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>frm2concetrado</t>
+  </si>
+  <si>
+    <t>cal_isr</t>
+  </si>
+  <si>
+    <t>cal_ietu</t>
+  </si>
+  <si>
+    <t>cal_iva</t>
+  </si>
+  <si>
+    <t>cal_ret</t>
+  </si>
+  <si>
+    <t>cal_ret1</t>
+  </si>
+  <si>
+    <t>cal_retiva</t>
+  </si>
+  <si>
+    <t>cal_nom</t>
+  </si>
+  <si>
+    <t>cal_hos</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -3350,7 +3386,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3766,9 +3802,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3895,54 +3928,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3958,6 +3943,58 @@
     <xf numFmtId="164" fontId="36" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="36" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Énfasis5" xfId="2" builtinId="47"/>
@@ -4375,138 +4412,138 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A2" s="252" t="s">
+      <c r="A2" s="264" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="252"/>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-      <c r="E2" s="252"/>
-      <c r="F2" s="252"/>
-      <c r="G2" s="252"/>
-      <c r="H2" s="252"/>
-      <c r="I2" s="252"/>
-      <c r="L2" s="253" t="s">
+      <c r="B2" s="264"/>
+      <c r="C2" s="264"/>
+      <c r="D2" s="264"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
+      <c r="L2" s="265" t="s">
         <v>350</v>
       </c>
-      <c r="M2" s="253"/>
-      <c r="N2" s="253"/>
-      <c r="O2" s="253"/>
-      <c r="P2" s="253"/>
-      <c r="Q2" s="253"/>
-      <c r="R2" s="253"/>
-      <c r="S2" s="253"/>
-      <c r="T2" s="253"/>
-      <c r="W2" s="254" t="s">
+      <c r="M2" s="265"/>
+      <c r="N2" s="265"/>
+      <c r="O2" s="265"/>
+      <c r="P2" s="265"/>
+      <c r="Q2" s="265"/>
+      <c r="R2" s="265"/>
+      <c r="S2" s="265"/>
+      <c r="T2" s="265"/>
+      <c r="W2" s="266" t="s">
         <v>350</v>
       </c>
-      <c r="X2" s="254"/>
-      <c r="Y2" s="254"/>
-      <c r="Z2" s="254"/>
-      <c r="AA2" s="254"/>
-      <c r="AB2" s="254"/>
-      <c r="AC2" s="254"/>
-      <c r="AD2" s="254"/>
-      <c r="AE2" s="254"/>
-      <c r="AF2" s="254"/>
-      <c r="AK2" s="246" t="s">
+      <c r="X2" s="266"/>
+      <c r="Y2" s="266"/>
+      <c r="Z2" s="266"/>
+      <c r="AA2" s="266"/>
+      <c r="AB2" s="266"/>
+      <c r="AC2" s="266"/>
+      <c r="AD2" s="266"/>
+      <c r="AE2" s="266"/>
+      <c r="AF2" s="266"/>
+      <c r="AK2" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="AL2" s="246"/>
-      <c r="AM2" s="246"/>
-      <c r="AN2" s="246"/>
-      <c r="AO2" s="246"/>
-      <c r="AP2" s="246"/>
-      <c r="AQ2" s="246"/>
-      <c r="AR2" s="246"/>
-      <c r="AS2" s="246"/>
-      <c r="AX2" s="246" t="s">
+      <c r="AL2" s="258"/>
+      <c r="AM2" s="258"/>
+      <c r="AN2" s="258"/>
+      <c r="AO2" s="258"/>
+      <c r="AP2" s="258"/>
+      <c r="AQ2" s="258"/>
+      <c r="AR2" s="258"/>
+      <c r="AS2" s="258"/>
+      <c r="AX2" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="AY2" s="246"/>
-      <c r="AZ2" s="246"/>
-      <c r="BA2" s="246"/>
-      <c r="BB2" s="246"/>
-      <c r="BC2" s="246"/>
-      <c r="BD2" s="246"/>
-      <c r="BE2" s="246"/>
-      <c r="BF2" s="246"/>
-      <c r="BG2" s="198"/>
+      <c r="AY2" s="258"/>
+      <c r="AZ2" s="258"/>
+      <c r="BA2" s="258"/>
+      <c r="BB2" s="258"/>
+      <c r="BC2" s="258"/>
+      <c r="BD2" s="258"/>
+      <c r="BE2" s="258"/>
+      <c r="BF2" s="258"/>
+      <c r="BG2" s="197"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A4" s="257" t="s">
+      <c r="A4" s="269" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="255" t="s">
+      <c r="B4" s="269"/>
+      <c r="C4" s="267" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="250"/>
-      <c r="E4" s="250"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="250"/>
-      <c r="H4" s="250"/>
-      <c r="I4" s="251"/>
+      <c r="D4" s="262"/>
+      <c r="E4" s="262"/>
+      <c r="F4" s="262"/>
+      <c r="G4" s="262"/>
+      <c r="H4" s="262"/>
+      <c r="I4" s="263"/>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
-      <c r="L4" s="260" t="s">
+      <c r="L4" s="272" t="s">
         <v>227</v>
       </c>
-      <c r="M4" s="261"/>
+      <c r="M4" s="273"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="255" t="s">
+      <c r="O4" s="267" t="s">
         <v>285</v>
       </c>
-      <c r="P4" s="250"/>
-      <c r="Q4" s="250"/>
-      <c r="R4" s="250"/>
-      <c r="S4" s="251"/>
+      <c r="P4" s="262"/>
+      <c r="Q4" s="262"/>
+      <c r="R4" s="262"/>
+      <c r="S4" s="263"/>
       <c r="T4" s="36"/>
       <c r="U4" s="36"/>
-      <c r="W4" s="258" t="s">
+      <c r="W4" s="270" t="s">
         <v>227</v>
       </c>
-      <c r="X4" s="258"/>
+      <c r="X4" s="270"/>
       <c r="Y4" s="68"/>
-      <c r="Z4" s="259" t="s">
+      <c r="Z4" s="271" t="s">
         <v>288</v>
       </c>
-      <c r="AA4" s="259"/>
-      <c r="AB4" s="259"/>
-      <c r="AC4" s="259"/>
-      <c r="AD4" s="259"/>
-      <c r="AE4" s="259"/>
-      <c r="AF4" s="259"/>
-      <c r="AK4" s="247" t="s">
+      <c r="AA4" s="271"/>
+      <c r="AB4" s="271"/>
+      <c r="AC4" s="271"/>
+      <c r="AD4" s="271"/>
+      <c r="AE4" s="271"/>
+      <c r="AF4" s="271"/>
+      <c r="AK4" s="259" t="s">
         <v>227</v>
       </c>
-      <c r="AL4" s="248"/>
+      <c r="AL4" s="260"/>
       <c r="AM4" s="78"/>
-      <c r="AN4" s="255" t="s">
+      <c r="AN4" s="267" t="s">
         <v>364</v>
       </c>
-      <c r="AO4" s="250"/>
-      <c r="AP4" s="250"/>
-      <c r="AQ4" s="250"/>
-      <c r="AR4" s="251"/>
+      <c r="AO4" s="262"/>
+      <c r="AP4" s="262"/>
+      <c r="AQ4" s="262"/>
+      <c r="AR4" s="263"/>
       <c r="AS4" s="78"/>
       <c r="AT4" s="78"/>
-      <c r="AX4" s="247" t="s">
+      <c r="AX4" s="259" t="s">
         <v>227</v>
       </c>
-      <c r="AY4" s="248"/>
+      <c r="AY4" s="260"/>
       <c r="AZ4" s="171"/>
-      <c r="BA4" s="249" t="s">
+      <c r="BA4" s="261" t="s">
         <v>561</v>
       </c>
-      <c r="BB4" s="250"/>
-      <c r="BC4" s="250"/>
-      <c r="BD4" s="250"/>
-      <c r="BE4" s="251"/>
+      <c r="BB4" s="262"/>
+      <c r="BC4" s="262"/>
+      <c r="BD4" s="262"/>
+      <c r="BE4" s="263"/>
       <c r="BF4" s="171"/>
-      <c r="BG4" s="198"/>
+      <c r="BG4" s="197"/>
       <c r="BJ4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="5" spans="1:62" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4651,8 +4688,8 @@
         <v>351</v>
       </c>
       <c r="BF5" s="82"/>
-      <c r="BG5" s="199"/>
-      <c r="BJ5" s="201">
+      <c r="BG5" s="198"/>
+      <c r="BJ5" s="200">
         <v>8000</v>
       </c>
     </row>
@@ -4761,7 +4798,7 @@
       <c r="BC6" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="BD6" s="194">
+      <c r="BD6" s="193">
         <v>9.9</v>
       </c>
       <c r="BE6" s="47" t="s">
@@ -4771,12 +4808,12 @@
         <v>253</v>
       </c>
       <c r="BG6" s="81" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="BH6" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="BI6" s="200">
+      <c r="BI6" s="199">
         <v>9000</v>
       </c>
     </row>
@@ -4893,7 +4930,7 @@
       <c r="BC7" s="172" t="s">
         <v>331</v>
       </c>
-      <c r="BD7" s="194">
+      <c r="BD7" s="193">
         <v>9.9</v>
       </c>
       <c r="BE7" s="47" t="s">
@@ -4903,12 +4940,12 @@
         <v>253</v>
       </c>
       <c r="BG7" s="81" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="BH7" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="BI7" s="200">
+      <c r="BI7" s="199">
         <v>3000</v>
       </c>
     </row>
@@ -4923,10 +4960,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="256" t="s">
+      <c r="E8" s="268" t="s">
         <v>308</v>
       </c>
-      <c r="F8" s="256"/>
+      <c r="F8" s="268"/>
       <c r="G8" s="14"/>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -5017,7 +5054,7 @@
         <v>6</v>
       </c>
       <c r="BC8" s="172"/>
-      <c r="BD8" s="194">
+      <c r="BD8" s="193">
         <v>9.9</v>
       </c>
       <c r="BE8" s="47" t="s">
@@ -5025,12 +5062,12 @@
       </c>
       <c r="BF8" s="72"/>
       <c r="BG8" s="81" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="BH8" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="BI8" s="200">
+      <c r="BI8" s="199">
         <f>IF(BI7&gt;=BI6,BI7-BI6,0)</f>
         <v>0</v>
       </c>
@@ -5140,7 +5177,7 @@
         <v>8</v>
       </c>
       <c r="BA9" s="108" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="BB9" s="81" t="s">
         <v>8</v>
@@ -5148,7 +5185,7 @@
       <c r="BC9" s="172" t="s">
         <v>332</v>
       </c>
-      <c r="BD9" s="194">
+      <c r="BD9" s="193">
         <v>9.9</v>
       </c>
       <c r="BE9" s="47" t="s">
@@ -5158,12 +5195,12 @@
         <v>253</v>
       </c>
       <c r="BG9" s="81" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="BH9" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="BI9" s="200">
+      <c r="BI9" s="199">
         <f>IF(BI6&gt;=BI7,IF(BJ5&gt;=BI6-BI7,BI6-BI7,BJ5),0)</f>
         <v>6000</v>
       </c>
@@ -5258,15 +5295,15 @@
         <v>9.9</v>
       </c>
       <c r="BE10" s="85" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="BG10" s="81" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="BH10" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="BI10" s="200">
+      <c r="BI10" s="199">
         <f>IF(BI9&lt;=0,BI8+BJ5,IF(BJ5&gt;=BI9,BJ5-BI9,0))</f>
         <v>2000</v>
       </c>
@@ -5369,7 +5406,7 @@
       <c r="AX11" s="72"/>
       <c r="AZ11" s="81"/>
       <c r="BA11" s="8" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="BB11" s="81" t="s">
         <v>12</v>
@@ -5386,7 +5423,7 @@
       <c r="BH11" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="BI11" s="200">
+      <c r="BI11" s="199">
         <f>IF(BI6&gt;=(BI7+BI9),BI6-(BI7+BI9),0)</f>
         <v>0</v>
       </c>
@@ -5497,14 +5534,14 @@
       <c r="BC12" s="172" t="s">
         <v>347</v>
       </c>
-      <c r="BD12" s="194">
+      <c r="BD12" s="193">
         <v>9.9</v>
       </c>
       <c r="BE12" s="85" t="s">
         <v>567</v>
       </c>
       <c r="BF12" s="72" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="BG12" s="72"/>
       <c r="BH12" s="81" t="s">
@@ -5607,7 +5644,7 @@
       <c r="BC13" s="172" t="s">
         <v>342</v>
       </c>
-      <c r="BD13" s="195">
+      <c r="BD13" s="194">
         <v>9.9900000000000003E-2</v>
       </c>
       <c r="BE13" s="47" t="s">
@@ -5708,7 +5745,7 @@
       <c r="AY14" s="17"/>
       <c r="AZ14" s="81"/>
       <c r="BA14" s="8" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="BB14" s="81" t="s">
         <v>18</v>
@@ -5819,7 +5856,7 @@
       <c r="AY15" s="17"/>
       <c r="AZ15" s="81"/>
       <c r="BA15" s="8" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="BB15" s="81" t="s">
         <v>20</v>
@@ -5950,7 +5987,7 @@
         <v>22</v>
       </c>
       <c r="BC16" s="172"/>
-      <c r="BD16" s="193">
+      <c r="BD16" s="192">
         <v>0.99990000000000001</v>
       </c>
       <c r="BE16" s="47" t="s">
@@ -6063,7 +6100,7 @@
         <v>24</v>
       </c>
       <c r="BC17" s="172"/>
-      <c r="BD17" s="193">
+      <c r="BD17" s="192">
         <v>0.99990000000000001</v>
       </c>
       <c r="BE17" s="47" t="s">
@@ -6170,7 +6207,7 @@
         <v>26</v>
       </c>
       <c r="BC18" s="172"/>
-      <c r="BD18" s="196">
+      <c r="BD18" s="195">
         <v>9.9</v>
       </c>
       <c r="BE18" s="72" t="s">
@@ -6271,13 +6308,13 @@
       <c r="AY19" s="17"/>
       <c r="AZ19" s="81"/>
       <c r="BA19" s="8" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="BB19" s="81" t="s">
         <v>28</v>
       </c>
       <c r="BC19" s="172"/>
-      <c r="BD19" s="196">
+      <c r="BD19" s="195">
         <v>9.9</v>
       </c>
       <c r="BE19" s="72" t="s">
@@ -6388,7 +6425,7 @@
       <c r="AY20" s="17"/>
       <c r="AZ20" s="81"/>
       <c r="BA20" s="8" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="BB20" s="81" t="s">
         <v>30</v>
@@ -6515,7 +6552,7 @@
         <v>31</v>
       </c>
       <c r="BC21" s="172"/>
-      <c r="BD21" s="195">
+      <c r="BD21" s="194">
         <v>9.9900000000000003E-2</v>
       </c>
       <c r="BE21" s="47" t="s">
@@ -6632,7 +6669,7 @@
         <v>33</v>
       </c>
       <c r="BC22" s="172"/>
-      <c r="BD22" s="194">
+      <c r="BD22" s="193">
         <v>9</v>
       </c>
       <c r="BE22" s="47" t="s">
@@ -6739,13 +6776,13 @@
       </c>
       <c r="AZ23" s="81"/>
       <c r="BA23" s="8" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="BB23" s="81" t="s">
         <v>35</v>
       </c>
       <c r="BC23" s="172"/>
-      <c r="BD23" s="195">
+      <c r="BD23" s="194">
         <v>9.9900000000000003E-2</v>
       </c>
       <c r="BE23" s="47" t="s">
@@ -6855,7 +6892,7 @@
       </c>
       <c r="AZ24" s="81"/>
       <c r="BA24" s="8" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="BB24" s="81" t="s">
         <v>36</v>
@@ -6973,7 +7010,7 @@
       </c>
       <c r="AZ25" s="81"/>
       <c r="BA25" s="8" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="BB25" s="81" t="s">
         <v>38</v>
@@ -7099,7 +7136,7 @@
       <c r="BC26" s="172" t="s">
         <v>303</v>
       </c>
-      <c r="BD26" s="194">
+      <c r="BD26" s="193">
         <v>9.9</v>
       </c>
       <c r="BE26" s="47" t="s">
@@ -7213,7 +7250,7 @@
       </c>
       <c r="AZ27" s="81"/>
       <c r="BA27" s="8" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="BB27" s="81" t="s">
         <v>41</v>
@@ -7327,7 +7364,7 @@
       </c>
       <c r="AZ28" s="81"/>
       <c r="BA28" s="8" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="BB28" s="81" t="s">
         <v>43</v>
@@ -7437,17 +7474,17 @@
       </c>
       <c r="AZ29" s="81"/>
       <c r="BA29" s="8" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="BB29" s="81" t="s">
-        <v>614</v>
-      </c>
-      <c r="BC29" s="197"/>
+        <v>608</v>
+      </c>
+      <c r="BC29" s="196"/>
       <c r="BD29" s="14">
         <v>9.9</v>
       </c>
       <c r="BE29" s="47" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="BF29" s="72"/>
       <c r="BG29" s="34"/>
@@ -9455,10 +9492,10 @@
       <c r="D52" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E52" s="256" t="s">
+      <c r="E52" s="268" t="s">
         <v>326</v>
       </c>
-      <c r="F52" s="256"/>
+      <c r="F52" s="268"/>
       <c r="G52" s="14"/>
       <c r="H52" s="5" t="s">
         <v>65</v>
@@ -9785,10 +9822,10 @@
       <c r="D56" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E56" s="256" t="s">
+      <c r="E56" s="268" t="s">
         <v>325</v>
       </c>
-      <c r="F56" s="256"/>
+      <c r="F56" s="268"/>
       <c r="G56" s="14"/>
       <c r="H56" s="5" t="s">
         <v>72</v>
@@ -10171,16 +10208,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="274" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="262"/>
+      <c r="B1" s="274"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
-      <c r="G1" s="262" t="s">
+      <c r="G1" s="274" t="s">
         <v>228</v>
       </c>
-      <c r="H1" s="262"/>
+      <c r="H1" s="274"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -13126,7 +13163,7 @@
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="204" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="203" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="42" style="94" customWidth="1"/>
@@ -13197,22 +13234,22 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="208" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="205"/>
-      <c r="B3" s="205"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="207" t="s">
+    <row r="3" spans="1:12" s="207" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="204"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="206" t="s">
         <v>187</v>
       </c>
       <c r="E3" s="104" t="s">
-        <v>645</v>
-      </c>
-      <c r="F3" s="233"/>
-      <c r="G3" s="234"/>
-      <c r="H3" s="235" t="s">
-        <v>617</v>
-      </c>
-      <c r="I3" s="236" t="s">
+        <v>639</v>
+      </c>
+      <c r="F3" s="232"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="234" t="s">
+        <v>611</v>
+      </c>
+      <c r="I3" s="235" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13348,10 +13385,10 @@
       <c r="B9" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="214" t="s">
+      <c r="C9" s="213" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="215" t="s">
+      <c r="D9" s="214" t="s">
         <v>199</v>
       </c>
       <c r="E9" s="104"/>
@@ -13371,10 +13408,10 @@
       <c r="B10" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="216" t="s">
+      <c r="C10" s="215" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="217" t="s">
+      <c r="D10" s="216" t="s">
         <v>201</v>
       </c>
       <c r="E10" s="104"/>
@@ -13387,20 +13424,20 @@
       </c>
       <c r="I10" s="106"/>
     </row>
-    <row r="11" spans="1:12" s="212" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="209"/>
-      <c r="B11" s="209"/>
-      <c r="C11" s="210"/>
-      <c r="D11" s="211" t="s">
+    <row r="11" spans="1:12" s="211" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="208"/>
+      <c r="B11" s="208"/>
+      <c r="C11" s="209"/>
+      <c r="D11" s="210" t="s">
         <v>203</v>
       </c>
       <c r="E11" s="104"/>
       <c r="F11" s="105" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G11" s="128"/>
       <c r="H11" s="47" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="I11" s="106"/>
     </row>
@@ -13411,15 +13448,15 @@
       <c r="B12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="214" t="s">
+      <c r="C12" s="213" t="s">
         <v>201</v>
       </c>
-      <c r="D12" s="215" t="s">
+      <c r="D12" s="214" t="s">
         <v>205</v>
       </c>
       <c r="E12" s="104"/>
       <c r="F12" s="105" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="G12" s="128"/>
       <c r="H12" s="47" t="s">
@@ -13434,15 +13471,15 @@
       <c r="B13" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="C13" s="216" t="s">
+      <c r="C13" s="215" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="217" t="s">
+      <c r="D13" s="216" t="s">
         <v>207</v>
       </c>
       <c r="E13" s="104"/>
       <c r="F13" s="105" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="G13" s="128"/>
       <c r="H13" s="47" t="s">
@@ -13457,15 +13494,15 @@
       <c r="B14" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="C14" s="218" t="s">
+      <c r="C14" s="217" t="s">
         <v>205</v>
       </c>
-      <c r="D14" s="219" t="s">
+      <c r="D14" s="218" t="s">
         <v>209</v>
       </c>
       <c r="E14" s="104"/>
       <c r="F14" s="105" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="G14" s="128"/>
       <c r="H14" s="47" t="s">
@@ -13480,15 +13517,15 @@
       <c r="B15" s="72" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="220" t="s">
+      <c r="C15" s="219" t="s">
         <v>207</v>
       </c>
-      <c r="D15" s="221" t="s">
+      <c r="D15" s="220" t="s">
         <v>211</v>
       </c>
       <c r="E15" s="104"/>
       <c r="F15" s="105" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="G15" s="128"/>
       <c r="H15" s="47" t="s">
@@ -13496,41 +13533,41 @@
       </c>
       <c r="I15" s="106"/>
     </row>
-    <row r="16" spans="1:12" s="212" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="209"/>
-      <c r="B16" s="209"/>
-      <c r="C16" s="210"/>
-      <c r="D16" s="211" t="s">
+    <row r="16" spans="1:12" s="211" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="208"/>
+      <c r="B16" s="208"/>
+      <c r="C16" s="209"/>
+      <c r="D16" s="210" t="s">
         <v>213</v>
       </c>
-      <c r="E16" s="237" t="s">
-        <v>646</v>
-      </c>
-      <c r="F16" s="238"/>
-      <c r="G16" s="239"/>
-      <c r="H16" s="240" t="s">
-        <v>619</v>
-      </c>
-      <c r="I16" s="241" t="s">
+      <c r="E16" s="236" t="s">
+        <v>640</v>
+      </c>
+      <c r="F16" s="237"/>
+      <c r="G16" s="238"/>
+      <c r="H16" s="239" t="s">
+        <v>613</v>
+      </c>
+      <c r="I16" s="240" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="212" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="209"/>
-      <c r="B17" s="209"/>
-      <c r="C17" s="210"/>
-      <c r="D17" s="211" t="s">
+    <row r="17" spans="1:12" s="211" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="208"/>
+      <c r="B17" s="208"/>
+      <c r="C17" s="209"/>
+      <c r="D17" s="210" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="237" t="s">
-        <v>647</v>
-      </c>
-      <c r="F17" s="238"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="240" t="s">
-        <v>620</v>
-      </c>
-      <c r="I17" s="241" t="s">
+      <c r="E17" s="236" t="s">
+        <v>641</v>
+      </c>
+      <c r="F17" s="237"/>
+      <c r="G17" s="238"/>
+      <c r="H17" s="239" t="s">
+        <v>614</v>
+      </c>
+      <c r="I17" s="240" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13547,17 +13584,17 @@
       <c r="D18" s="120" t="s">
         <v>216</v>
       </c>
-      <c r="E18" s="226"/>
-      <c r="F18" s="227" t="s">
-        <v>626</v>
-      </c>
-      <c r="G18" s="228">
+      <c r="E18" s="225"/>
+      <c r="F18" s="226" t="s">
+        <v>620</v>
+      </c>
+      <c r="G18" s="227">
         <v>9.99</v>
       </c>
-      <c r="H18" s="229" t="s">
+      <c r="H18" s="228" t="s">
         <v>273</v>
       </c>
-      <c r="I18" s="230"/>
+      <c r="I18" s="229"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
@@ -13596,23 +13633,23 @@
       <c r="B20" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="214" t="s">
+      <c r="C20" s="213" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="215" t="s">
+      <c r="D20" s="214" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="222"/>
-      <c r="F20" s="223" t="s">
-        <v>627</v>
-      </c>
-      <c r="G20" s="228">
+      <c r="E20" s="221"/>
+      <c r="F20" s="222" t="s">
+        <v>621</v>
+      </c>
+      <c r="G20" s="227">
         <v>9.99</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="I20" s="224"/>
+      <c r="I20" s="223"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
@@ -13638,23 +13675,23 @@
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="72"/>
       <c r="B22" s="72"/>
-      <c r="C22" s="216" t="s">
+      <c r="C22" s="215" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="217" t="s">
+      <c r="D22" s="216" t="s">
         <v>222</v>
       </c>
-      <c r="E22" s="222"/>
-      <c r="F22" s="223" t="s">
-        <v>628</v>
-      </c>
-      <c r="G22" s="228">
+      <c r="E22" s="221"/>
+      <c r="F22" s="222" t="s">
+        <v>622</v>
+      </c>
+      <c r="G22" s="227">
         <v>9.99</v>
       </c>
       <c r="H22" s="28" t="s">
         <v>387</v>
       </c>
-      <c r="I22" s="224"/>
+      <c r="I22" s="223"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="72"/>
@@ -13680,23 +13717,23 @@
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="72"/>
       <c r="B24" s="72"/>
-      <c r="C24" s="218" t="s">
+      <c r="C24" s="217" t="s">
         <v>219</v>
       </c>
-      <c r="D24" s="219" t="s">
+      <c r="D24" s="218" t="s">
         <v>224</v>
       </c>
-      <c r="E24" s="222"/>
-      <c r="F24" s="223" t="s">
-        <v>629</v>
-      </c>
-      <c r="G24" s="228">
+      <c r="E24" s="221"/>
+      <c r="F24" s="222" t="s">
+        <v>623</v>
+      </c>
+      <c r="G24" s="227">
         <v>9.99</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>389</v>
       </c>
-      <c r="I24" s="224"/>
+      <c r="I24" s="223"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="72"/>
@@ -13722,23 +13759,23 @@
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="72"/>
       <c r="B26" s="72"/>
-      <c r="C26" s="220" t="s">
+      <c r="C26" s="219" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="221" t="s">
+      <c r="D26" s="220" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="222"/>
-      <c r="F26" s="223" t="s">
-        <v>630</v>
-      </c>
-      <c r="G26" s="228">
+      <c r="E26" s="221"/>
+      <c r="F26" s="222" t="s">
+        <v>624</v>
+      </c>
+      <c r="G26" s="227">
         <v>9.99</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>391</v>
       </c>
-      <c r="I26" s="224"/>
+      <c r="I26" s="223"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="72"/>
@@ -13770,17 +13807,17 @@
       <c r="D28" s="120" t="s">
         <v>399</v>
       </c>
-      <c r="E28" s="222"/>
-      <c r="F28" s="223" t="s">
-        <v>631</v>
-      </c>
-      <c r="G28" s="228">
+      <c r="E28" s="221"/>
+      <c r="F28" s="222" t="s">
+        <v>625</v>
+      </c>
+      <c r="G28" s="227">
         <v>9.99</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>393</v>
       </c>
-      <c r="I28" s="224"/>
+      <c r="I28" s="223"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="72"/>
@@ -13812,17 +13849,17 @@
       <c r="D30" s="120" t="s">
         <v>403</v>
       </c>
-      <c r="E30" s="226"/>
-      <c r="F30" s="223" t="s">
-        <v>632</v>
-      </c>
-      <c r="G30" s="228">
+      <c r="E30" s="225"/>
+      <c r="F30" s="222" t="s">
+        <v>626</v>
+      </c>
+      <c r="G30" s="227">
         <v>9.99</v>
       </c>
-      <c r="H30" s="229" t="s">
+      <c r="H30" s="228" t="s">
         <v>395</v>
       </c>
-      <c r="I30" s="230"/>
+      <c r="I30" s="229"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
@@ -13863,17 +13900,17 @@
       <c r="D32" s="120" t="s">
         <v>407</v>
       </c>
-      <c r="E32" s="222"/>
-      <c r="F32" s="223" t="s">
-        <v>633</v>
-      </c>
-      <c r="G32" s="228">
+      <c r="E32" s="221"/>
+      <c r="F32" s="222" t="s">
+        <v>627</v>
+      </c>
+      <c r="G32" s="227">
         <v>9.99</v>
       </c>
       <c r="H32" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="I32" s="224"/>
+      <c r="I32" s="223"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="72"/>
@@ -13886,24 +13923,24 @@
       <c r="D33" s="120" t="s">
         <v>408</v>
       </c>
-      <c r="E33" s="222"/>
-      <c r="F33" s="223" t="s">
-        <v>634</v>
-      </c>
-      <c r="G33" s="228">
+      <c r="E33" s="221"/>
+      <c r="F33" s="222" t="s">
+        <v>628</v>
+      </c>
+      <c r="G33" s="227">
         <v>9.99</v>
       </c>
       <c r="H33" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="I33" s="224"/>
-      <c r="N33" s="203" t="s">
+      <c r="I33" s="223"/>
+      <c r="N33" s="202" t="s">
         <v>526</v>
       </c>
-      <c r="O33" s="203" t="s">
+      <c r="O33" s="202" t="s">
         <v>527</v>
       </c>
-      <c r="P33" s="203" t="s">
+      <c r="P33" s="202" t="s">
         <v>528</v>
       </c>
     </row>
@@ -13918,17 +13955,17 @@
       <c r="D34" s="120" t="s">
         <v>409</v>
       </c>
-      <c r="E34" s="222"/>
-      <c r="F34" s="223" t="s">
-        <v>635</v>
-      </c>
-      <c r="G34" s="225">
+      <c r="E34" s="221"/>
+      <c r="F34" s="222" t="s">
+        <v>629</v>
+      </c>
+      <c r="G34" s="224">
         <v>9.99</v>
       </c>
       <c r="H34" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="I34" s="224"/>
+      <c r="I34" s="223"/>
       <c r="J34" s="124" t="s">
         <v>403</v>
       </c>
@@ -13939,9 +13976,9 @@
       <c r="M34" s="160" t="s">
         <v>405</v>
       </c>
-      <c r="N34" s="203"/>
-      <c r="O34" s="203"/>
-      <c r="P34" s="203"/>
+      <c r="N34" s="202"/>
+      <c r="O34" s="202"/>
+      <c r="P34" s="202"/>
       <c r="Q34" s="124" t="s">
         <v>403</v>
       </c>
@@ -13978,9 +14015,9 @@
       <c r="M35" s="161" t="s">
         <v>162</v>
       </c>
-      <c r="N35" s="203"/>
-      <c r="O35" s="203"/>
-      <c r="P35" s="203"/>
+      <c r="N35" s="202"/>
+      <c r="O35" s="202"/>
+      <c r="P35" s="202"/>
       <c r="Q35" s="124" t="s">
         <v>406</v>
       </c>
@@ -14017,9 +14054,9 @@
       <c r="M36" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="N36" s="203"/>
-      <c r="O36" s="203"/>
-      <c r="P36" s="203"/>
+      <c r="N36" s="202"/>
+      <c r="O36" s="202"/>
+      <c r="P36" s="202"/>
       <c r="Q36" s="124" t="s">
         <v>407</v>
       </c>
@@ -14033,17 +14070,17 @@
       <c r="D37" s="120" t="s">
         <v>413</v>
       </c>
-      <c r="E37" s="222"/>
-      <c r="F37" s="231" t="s">
-        <v>636</v>
-      </c>
-      <c r="G37" s="228">
+      <c r="E37" s="221"/>
+      <c r="F37" s="230" t="s">
+        <v>630</v>
+      </c>
+      <c r="G37" s="227">
         <v>9.99</v>
       </c>
       <c r="H37" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="I37" s="224"/>
+      <c r="I37" s="223"/>
       <c r="J37" s="124" t="s">
         <v>408</v>
       </c>
@@ -14054,13 +14091,13 @@
       <c r="M37" s="162" t="s">
         <v>402</v>
       </c>
-      <c r="N37" s="203">
+      <c r="N37" s="202">
         <v>0</v>
       </c>
-      <c r="O37" s="203">
+      <c r="O37" s="202">
         <v>1316.56</v>
       </c>
-      <c r="P37" s="203"/>
+      <c r="P37" s="202"/>
       <c r="Q37" s="124" t="s">
         <v>408</v>
       </c>
@@ -14074,17 +14111,17 @@
       <c r="D38" s="120" t="s">
         <v>414</v>
       </c>
-      <c r="E38" s="222"/>
-      <c r="F38" s="232" t="s">
-        <v>637</v>
-      </c>
-      <c r="G38" s="225">
+      <c r="E38" s="221"/>
+      <c r="F38" s="231" t="s">
+        <v>631</v>
+      </c>
+      <c r="G38" s="224">
         <v>9.99</v>
       </c>
       <c r="H38" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="I38" s="224"/>
+      <c r="I38" s="223"/>
       <c r="J38" s="124" t="s">
         <v>409</v>
       </c>
@@ -14095,13 +14132,13 @@
       <c r="M38" s="162" t="s">
         <v>405</v>
       </c>
-      <c r="N38" s="203">
+      <c r="N38" s="202">
         <v>3148.07</v>
       </c>
-      <c r="O38" s="203">
+      <c r="O38" s="202">
         <v>0</v>
       </c>
-      <c r="P38" s="203">
+      <c r="P38" s="202">
         <v>2189.7399999999998</v>
       </c>
       <c r="Q38" s="124" t="s">
@@ -14121,7 +14158,7 @@
         <v>424</v>
       </c>
       <c r="F39" s="108" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="G39" s="133"/>
       <c r="H39" s="109" t="s">
@@ -14142,14 +14179,14 @@
       <c r="M39" s="163" t="s">
         <v>524</v>
       </c>
-      <c r="N39" s="203">
+      <c r="N39" s="202">
         <v>0</v>
       </c>
-      <c r="O39" s="203">
+      <c r="O39" s="202">
         <f>+N41</f>
         <v>3148.07</v>
       </c>
-      <c r="P39" s="203">
+      <c r="P39" s="202">
         <f>+O42</f>
         <v>1831.5100000000002</v>
       </c>
@@ -14171,13 +14208,13 @@
       <c r="M40" s="163" t="s">
         <v>411</v>
       </c>
-      <c r="N40" s="203">
+      <c r="N40" s="202">
         <v>0</v>
       </c>
-      <c r="O40" s="203">
+      <c r="O40" s="202">
         <v>1316.56</v>
       </c>
-      <c r="P40" s="203">
+      <c r="P40" s="202">
         <v>0</v>
       </c>
       <c r="Q40" s="124" t="s">
@@ -14198,15 +14235,15 @@
       <c r="M41" s="164" t="s">
         <v>525</v>
       </c>
-      <c r="N41" s="203">
+      <c r="N41" s="202">
         <f>+N38</f>
         <v>3148.07</v>
       </c>
-      <c r="O41" s="203">
+      <c r="O41" s="202">
         <f>+O38</f>
         <v>0</v>
       </c>
-      <c r="P41" s="203">
+      <c r="P41" s="202">
         <f>+P38+P39</f>
         <v>4021.25</v>
       </c>
@@ -14225,7 +14262,7 @@
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="97" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="G42" s="130">
         <v>9.99</v>
@@ -14246,14 +14283,14 @@
       <c r="M42" s="165" t="s">
         <v>402</v>
       </c>
-      <c r="N42" s="203">
+      <c r="N42" s="202">
         <v>0</v>
       </c>
-      <c r="O42" s="203">
+      <c r="O42" s="202">
         <f>+O39-O40</f>
         <v>1831.5100000000002</v>
       </c>
-      <c r="P42" s="203">
+      <c r="P42" s="202">
         <f>+P37-P40</f>
         <v>0</v>
       </c>
@@ -14297,9 +14334,9 @@
       <c r="M43" s="161" t="s">
         <v>168</v>
       </c>
-      <c r="N43" s="203"/>
-      <c r="O43" s="203"/>
-      <c r="P43" s="203"/>
+      <c r="N43" s="202"/>
+      <c r="O43" s="202"/>
+      <c r="P43" s="202"/>
       <c r="Q43" s="124" t="s">
         <v>415</v>
       </c>
@@ -14340,9 +14377,9 @@
       <c r="M44" s="161" t="s">
         <v>170</v>
       </c>
-      <c r="N44" s="203"/>
-      <c r="O44" s="203"/>
-      <c r="P44" s="203"/>
+      <c r="N44" s="202"/>
+      <c r="O44" s="202"/>
+      <c r="P44" s="202"/>
       <c r="Q44" s="111" t="s">
         <v>416</v>
       </c>
@@ -14360,7 +14397,7 @@
       <c r="D45" s="124" t="s">
         <v>419</v>
       </c>
-      <c r="E45" s="202"/>
+      <c r="E45" s="201"/>
       <c r="F45" s="95" t="s">
         <v>296</v>
       </c>
@@ -14383,9 +14420,9 @@
       <c r="M45" s="166" t="s">
         <v>218</v>
       </c>
-      <c r="N45" s="203"/>
-      <c r="O45" s="203"/>
-      <c r="P45" s="203"/>
+      <c r="N45" s="202"/>
+      <c r="O45" s="202"/>
+      <c r="P45" s="202"/>
       <c r="Q45" s="111" t="s">
         <v>417</v>
       </c>
@@ -14403,7 +14440,7 @@
       <c r="D46" s="124" t="s">
         <v>420</v>
       </c>
-      <c r="E46" s="202"/>
+      <c r="E46" s="201"/>
       <c r="F46" s="95" t="s">
         <v>296</v>
       </c>
@@ -14424,9 +14461,9 @@
       <c r="M46" s="166" t="s">
         <v>220</v>
       </c>
-      <c r="N46" s="203"/>
-      <c r="O46" s="203"/>
-      <c r="P46" s="203"/>
+      <c r="N46" s="202"/>
+      <c r="O46" s="202"/>
+      <c r="P46" s="202"/>
       <c r="Q46" s="111" t="s">
         <v>418</v>
       </c>
@@ -14461,15 +14498,15 @@
         <v>419</v>
       </c>
       <c r="K47" s="124" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="L47" s="111"/>
       <c r="M47" s="160" t="s">
         <v>175</v>
       </c>
-      <c r="N47" s="203"/>
-      <c r="O47" s="203"/>
-      <c r="P47" s="203"/>
+      <c r="N47" s="202"/>
+      <c r="O47" s="202"/>
+      <c r="P47" s="202"/>
       <c r="Q47" s="111" t="s">
         <v>419</v>
       </c>
@@ -14504,15 +14541,15 @@
         <v>420</v>
       </c>
       <c r="K48" s="124" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="L48" s="111"/>
       <c r="M48" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="N48" s="203"/>
-      <c r="O48" s="203"/>
-      <c r="P48" s="203"/>
+      <c r="N48" s="202"/>
+      <c r="O48" s="202"/>
+      <c r="P48" s="202"/>
       <c r="Q48" s="111" t="s">
         <v>420</v>
       </c>
@@ -14528,7 +14565,7 @@
         <v>419</v>
       </c>
       <c r="D49" s="124" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="E49" s="52"/>
       <c r="F49" s="105" t="s">
@@ -14545,15 +14582,15 @@
         <v>421</v>
       </c>
       <c r="K49" s="124" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="L49" s="111"/>
       <c r="M49" s="161" t="s">
         <v>179</v>
       </c>
-      <c r="N49" s="203"/>
-      <c r="O49" s="203"/>
-      <c r="P49" s="203"/>
+      <c r="N49" s="202"/>
+      <c r="O49" s="202"/>
+      <c r="P49" s="202"/>
       <c r="Q49" s="111" t="s">
         <v>421</v>
       </c>
@@ -14569,9 +14606,9 @@
         <v>420</v>
       </c>
       <c r="D50" s="124" t="s">
-        <v>640</v>
-      </c>
-      <c r="E50" s="202"/>
+        <v>634</v>
+      </c>
+      <c r="E50" s="201"/>
       <c r="F50" s="95" t="s">
         <v>296</v>
       </c>
@@ -14588,15 +14625,15 @@
         <v>422</v>
       </c>
       <c r="K50" s="124" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="L50" s="111"/>
       <c r="M50" s="166" t="s">
         <v>59</v>
       </c>
-      <c r="N50" s="203"/>
-      <c r="O50" s="203"/>
-      <c r="P50" s="203"/>
+      <c r="N50" s="202"/>
+      <c r="O50" s="202"/>
+      <c r="P50" s="202"/>
       <c r="Q50" s="111" t="s">
         <v>422</v>
       </c>
@@ -14608,11 +14645,11 @@
       <c r="B51" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="204" t="s">
+      <c r="C51" s="203" t="s">
         <v>421</v>
       </c>
       <c r="D51" s="124" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="E51" s="144"/>
       <c r="F51" s="143" t="s">
@@ -14631,15 +14668,15 @@
         <v>529</v>
       </c>
       <c r="K51" s="124" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="L51" s="111"/>
       <c r="M51" s="160" t="s">
         <v>61</v>
       </c>
-      <c r="N51" s="203"/>
-      <c r="O51" s="203"/>
-      <c r="P51" s="203"/>
+      <c r="N51" s="202"/>
+      <c r="O51" s="202"/>
+      <c r="P51" s="202"/>
       <c r="Q51" s="111" t="s">
         <v>529</v>
       </c>
@@ -14651,15 +14688,15 @@
       <c r="B52" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="204" t="s">
+      <c r="C52" s="203" t="s">
         <v>422</v>
       </c>
       <c r="D52" s="124" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="E52" s="144"/>
       <c r="F52" s="143" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="G52" s="138">
         <v>9.99</v>
@@ -14674,24 +14711,24 @@
         <v>530</v>
       </c>
       <c r="K52" s="124" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="L52" s="167"/>
       <c r="M52" s="160" t="s">
         <v>63</v>
       </c>
-      <c r="N52" s="203"/>
-      <c r="O52" s="203"/>
-      <c r="P52" s="203"/>
+      <c r="N52" s="202"/>
+      <c r="O52" s="202"/>
+      <c r="P52" s="202"/>
       <c r="Q52" s="167" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="204" t="s">
+      <c r="A53" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="B53" s="204"/>
+      <c r="B53" s="203"/>
       <c r="F53" s="158" t="s">
         <v>228</v>
       </c>
@@ -15495,7 +15532,7 @@
       <c r="E6" s="120" t="s">
         <v>193</v>
       </c>
-      <c r="F6" s="191" t="s">
+      <c r="F6" s="190" t="s">
         <v>303</v>
       </c>
       <c r="G6" s="188" t="s">
@@ -15542,7 +15579,7 @@
         <v>197</v>
       </c>
       <c r="F8" s="104"/>
-      <c r="G8" s="192" t="s">
+      <c r="G8" s="191" t="s">
         <v>578</v>
       </c>
       <c r="H8" s="106"/>
@@ -15584,7 +15621,7 @@
         <v>201</v>
       </c>
       <c r="F10" s="104"/>
-      <c r="G10" s="192" t="s">
+      <c r="G10" s="191" t="s">
         <v>553</v>
       </c>
       <c r="H10" s="106"/>
@@ -15604,7 +15641,7 @@
         <v>203</v>
       </c>
       <c r="F11" s="104"/>
-      <c r="G11" s="192" t="s">
+      <c r="G11" s="191" t="s">
         <v>186</v>
       </c>
       <c r="H11" s="106"/>
@@ -15633,7 +15670,7 @@
         <v>205</v>
       </c>
       <c r="F12" s="104"/>
-      <c r="G12" s="192" t="s">
+      <c r="G12" s="191" t="s">
         <v>555</v>
       </c>
       <c r="H12" s="106"/>
@@ -15651,7 +15688,7 @@
         <v>207</v>
       </c>
       <c r="F13" s="104"/>
-      <c r="G13" s="192" t="s">
+      <c r="G13" s="191" t="s">
         <v>554</v>
       </c>
       <c r="H13" s="106"/>
@@ -15666,7 +15703,7 @@
       </c>
       <c r="C14" s="104"/>
       <c r="D14" s="105" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="E14" s="120" t="s">
         <v>209</v>
@@ -15690,7 +15727,7 @@
       <c r="B15" s="120"/>
       <c r="C15" s="104"/>
       <c r="D15" s="105" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="E15" s="120" t="s">
         <v>211</v>
@@ -15707,7 +15744,7 @@
       <c r="B16" s="120"/>
       <c r="C16" s="104"/>
       <c r="D16" s="187" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="E16" s="120" t="s">
         <v>213</v>
@@ -15726,7 +15763,7 @@
       </c>
       <c r="C17" s="104"/>
       <c r="D17" s="105" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="E17" s="120" t="s">
         <v>215</v>
@@ -15736,7 +15773,7 @@
         <v>557</v>
       </c>
       <c r="H17" s="106"/>
-      <c r="I17" s="190">
+      <c r="I17" s="189">
         <v>38</v>
       </c>
       <c r="K17" s="185">
@@ -15761,7 +15798,7 @@
         <v>168</v>
       </c>
       <c r="H18" s="106"/>
-      <c r="I18" s="190">
+      <c r="I18" s="189">
         <v>39</v>
       </c>
       <c r="K18" s="182"/>
@@ -15782,7 +15819,7 @@
         <v>170</v>
       </c>
       <c r="H19" s="106"/>
-      <c r="I19" s="190">
+      <c r="I19" s="189">
         <v>40</v>
       </c>
       <c r="K19" s="182">
@@ -15806,7 +15843,7 @@
         <v>83</v>
       </c>
       <c r="H20" s="106"/>
-      <c r="I20" s="190">
+      <c r="I20" s="189">
         <v>41</v>
       </c>
       <c r="K20" s="182">
@@ -15830,7 +15867,7 @@
         <v>220</v>
       </c>
       <c r="H21" s="106"/>
-      <c r="I21" s="190">
+      <c r="I21" s="189">
         <v>42</v>
       </c>
       <c r="K21" s="185">
@@ -15854,7 +15891,7 @@
         <v>175</v>
       </c>
       <c r="H22" s="106"/>
-      <c r="I22" s="190">
+      <c r="I22" s="189">
         <v>43</v>
       </c>
     </row>
@@ -15874,7 +15911,7 @@
         <v>177</v>
       </c>
       <c r="H23" s="106"/>
-      <c r="I23" s="190">
+      <c r="I23" s="189">
         <v>44</v>
       </c>
     </row>
@@ -15894,7 +15931,7 @@
         <v>179</v>
       </c>
       <c r="H24" s="106"/>
-      <c r="I24" s="190">
+      <c r="I24" s="189">
         <v>45</v>
       </c>
     </row>
@@ -15914,7 +15951,7 @@
         <v>59</v>
       </c>
       <c r="H25" s="106"/>
-      <c r="I25" s="190">
+      <c r="I25" s="189">
         <v>46</v>
       </c>
     </row>
@@ -15934,7 +15971,7 @@
         <v>61</v>
       </c>
       <c r="H26" s="106"/>
-      <c r="I26" s="190">
+      <c r="I26" s="189">
         <v>47</v>
       </c>
     </row>
@@ -15954,7 +15991,7 @@
         <v>63</v>
       </c>
       <c r="H27" s="106"/>
-      <c r="I27" s="190">
+      <c r="I27" s="189">
         <v>48</v>
       </c>
     </row>
@@ -15991,145 +16028,156 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:I10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="189" t="s">
-        <v>585</v>
-      </c>
-      <c r="C2" s="189" t="s">
-        <v>586</v>
-      </c>
-      <c r="D2" s="189" t="s">
-        <v>589</v>
-      </c>
-      <c r="E2" s="189" t="s">
-        <v>587</v>
-      </c>
-      <c r="F2" s="189" t="s">
-        <v>588</v>
-      </c>
-      <c r="G2" s="189" t="s">
-        <v>590</v>
-      </c>
-      <c r="I2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>562</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>666</v>
       </c>
       <c r="B3">
-        <v>5000</v>
-      </c>
-      <c r="C3">
-        <v>3000</v>
+        <v>52</v>
+      </c>
+      <c r="C3" s="245" t="s">
+        <v>674</v>
       </c>
       <c r="D3">
-        <f>+B3+C3</f>
-        <v>8000</v>
-      </c>
-      <c r="E3">
-        <v>2500</v>
-      </c>
-      <c r="F3">
-        <v>4000</v>
-      </c>
-      <c r="G3">
-        <f>+E3+F3</f>
-        <v>6500</v>
-      </c>
-      <c r="I3">
-        <f>+B3+C3</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>563</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>667</v>
       </c>
       <c r="B4">
-        <v>7000</v>
-      </c>
-      <c r="C4">
-        <v>3000</v>
-      </c>
-      <c r="D4">
-        <f>+B4+C4</f>
-        <v>10000</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4">
-        <v>2000</v>
-      </c>
-      <c r="G4">
-        <f>+E4+F4</f>
-        <v>3000</v>
-      </c>
-      <c r="I4">
-        <f>+B4+C4</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>564</v>
+        <v>63</v>
+      </c>
+      <c r="C4" s="245" t="s">
+        <v>681</v>
+      </c>
+      <c r="F4" s="275">
+        <v>67383.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5" s="245" t="s">
+        <v>678</v>
       </c>
       <c r="D5">
-        <f>+D4-D3</f>
-        <v>2000</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>565</v>
-      </c>
-      <c r="G6">
-        <f>+D5</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
-        <v>566</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f>+G3-G4-G6</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>569</v>
+        <v>53</v>
+      </c>
+      <c r="F5">
+        <v>1267383.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>669</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" s="245" t="s">
+        <v>675</v>
+      </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" s="245"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>670</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" s="245" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>670</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9" s="245"/>
+      <c r="D9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>671</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10" s="245" t="s">
+        <v>679</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>672</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" s="245" t="s">
+        <v>676</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>673</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="245" t="s">
+        <v>677</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -16142,7 +16190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D6352A-C30E-4FA2-BEF1-5CC43B7B90A8}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -16154,71 +16202,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="243">
+      <c r="B1" s="242">
         <v>44562</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="213" t="s">
-        <v>654</v>
-      </c>
-      <c r="B2" s="263">
+      <c r="A2" s="212" t="s">
+        <v>648</v>
+      </c>
+      <c r="B2" s="246">
         <v>16074</v>
       </c>
-      <c r="C2" s="242" t="s">
+      <c r="C2" s="241" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="212" t="s">
+        <v>649</v>
+      </c>
+      <c r="B3" s="247">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="212" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="213" t="s">
-        <v>655</v>
-      </c>
-      <c r="B3" s="264">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="213" t="s">
-        <v>656</v>
-      </c>
-      <c r="B4" s="272">
+      <c r="B4" s="255">
         <f>+B2*B3</f>
         <v>401.85</v>
       </c>
-      <c r="C4" s="242" t="s">
+      <c r="C4" s="241" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="212" t="s">
+        <v>651</v>
+      </c>
+      <c r="B5" s="248">
+        <v>124.571</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="212" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="213" t="s">
-        <v>657</v>
-      </c>
-      <c r="B5" s="265">
-        <v>124.571</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="213" t="s">
-        <v>658</v>
-      </c>
-      <c r="B6" s="265">
+      <c r="B6" s="248">
         <v>118.002</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="213" t="s">
-        <v>659</v>
-      </c>
-      <c r="B7" s="266">
+      <c r="A7" s="212" t="s">
+        <v>653</v>
+      </c>
+      <c r="B7" s="249">
         <f>+B5/B6</f>
         <v>1.055668547990712</v>
       </c>
@@ -16227,42 +16275,42 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="213" t="s">
-        <v>660</v>
-      </c>
-      <c r="B8" s="274">
+      <c r="A8" s="212" t="s">
+        <v>654</v>
+      </c>
+      <c r="B8" s="257">
         <f>+B4*B7</f>
         <v>424.22040601006762</v>
       </c>
-      <c r="C8" s="242" t="s">
-        <v>668</v>
+      <c r="C8" s="241" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="213"/>
-      <c r="B9" s="267">
+      <c r="A9" s="212"/>
+      <c r="B9" s="250">
         <f>+B4</f>
         <v>401.85</v>
       </c>
-      <c r="C9" s="242" t="s">
-        <v>669</v>
+      <c r="C9" s="241" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="213"/>
-      <c r="B10" s="267">
+      <c r="A10" s="212"/>
+      <c r="B10" s="250">
         <f>+B8-B9</f>
         <v>22.370406010067597</v>
       </c>
-      <c r="C10" s="242" t="s">
-        <v>653</v>
+      <c r="C10" s="241" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="213" t="s">
-        <v>661</v>
-      </c>
-      <c r="B11" s="268">
+      <c r="A11" s="212" t="s">
+        <v>655</v>
+      </c>
+      <c r="B11" s="251">
         <v>1.47E-2</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -16270,10 +16318,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="213" t="s">
-        <v>662</v>
-      </c>
-      <c r="B12" s="269">
+      <c r="A12" s="212" t="s">
+        <v>656</v>
+      </c>
+      <c r="B12" s="252">
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
@@ -16281,10 +16329,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="213" t="s">
-        <v>663</v>
-      </c>
-      <c r="B13" s="270">
+      <c r="A13" s="212" t="s">
+        <v>657</v>
+      </c>
+      <c r="B13" s="253">
         <f>+B12*B11</f>
         <v>0.1323</v>
       </c>
@@ -16293,10 +16341,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="213" t="s">
-        <v>664</v>
-      </c>
-      <c r="B14" s="273">
+      <c r="A14" s="212" t="s">
+        <v>658</v>
+      </c>
+      <c r="B14" s="256">
         <f>+B4*B13</f>
         <v>53.164755000000007</v>
       </c>
@@ -16305,25 +16353,25 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="213" t="s">
-        <v>665</v>
-      </c>
-      <c r="B15" s="271">
+      <c r="A15" s="212" t="s">
+        <v>659</v>
+      </c>
+      <c r="B15" s="254">
         <f>+B4+B10+B14</f>
         <v>477.38516101006763</v>
       </c>
-      <c r="C15" s="242" t="s">
+      <c r="C15" s="241" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="244">
+      <c r="B17" s="243">
         <f>+B4</f>
         <v>401.85</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="245">
+      <c r="B18" s="244">
         <f>+B10</f>
         <v>22.370406010067597</v>
       </c>

</xml_diff>

<commit_message>
Cambios Calculo retenciones Personal moral
</commit_message>
<xml_diff>
--- a/Calculos_2015.xlsx
+++ b/Calculos_2015.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dtax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D097970B-ADE3-48D5-8FAC-A41BDBD1A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2D2654-C8DA-49D5-A25C-9FC53F5F9023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="717" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="783">
   <si>
     <t>clave</t>
   </si>
@@ -2585,6 +2585,309 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>Enterado</t>
+  </si>
+  <si>
+    <t>Contrubucion</t>
+  </si>
+  <si>
+    <t>*!*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       ******************************           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Calculo de Impuestos sobre nomina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>*//SELECT cap_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            *//SET FILTER TO ((anio=localejercicio) AND (id_em=nid_empresa))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            *//GO top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            *//i=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            *//DO WHILE i&lt;13   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            SELECT cal_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            GO top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            *// replace N1 Total Base gravable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                mes_de_pago[5,i]=cap_nom.mdp            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                paso= meses[i]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH cap_nom.k1+cap_nom.k2+cap_nom.k3  &amp;&amp;sueldos_sal+asimilables+otros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N2  tasa impuesto sobre Nomina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  IF sw5=.f.                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    tasa_de_n=0</t>
+  </si>
+  <si>
+    <t>SELECT  tasa_nomina</t>
+  </si>
+  <si>
+    <t>SET ORDER TO id_anio</t>
+  </si>
+  <si>
+    <t>SEEK localejercicio</t>
+  </si>
+  <si>
+    <t>IF FOUND()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tasa_de_n=tasa_nomina.tarifa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ENDIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                sw5=.t.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            endif                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SELECT cal_nom              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH  tasa_de_n      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N3  Impuesto sobre nomina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N3",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N4   INPC Mes Anterior Conocida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor= thisform.inpc_anterior(1,cap_nom.mdp,i,1,5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N5  INPC Mes Pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor= thisform.inpc_anterior(localejercicio,cap_nom.mdp,i,2,5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N6  Factor de Actualizacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N6",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N7  Impueso Propio de la Actividad Actualizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N7",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N8  Tasa de recargos por moratorios                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                IF sw6=.f.                  </t>
+  </si>
+  <si>
+    <t>SELECT  recargos</t>
+  </si>
+  <si>
+    <t>GO top</t>
+  </si>
+  <si>
+    <t>SET ORDER TO anio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SELECT cal_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.ene WITH  recargos.ene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.feb WITH  recargos.feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.mar WITH  recargos.mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.abr WITH  recargos.abr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.may WITH  recargos.may</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.jun WITH  recargos.jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.jul WITH  recargos.jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.ago WITH  recargos.ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.sep WITH  recargos.sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  REPLACE cal_nom.oct WITH  recargos.oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.nov WITH  recargos.nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  REPLACE cal_nom.dic WITH  recargos.dic            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                sw6=.t.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            ENDIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SELECT cal_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N9 Numero Meses trascurridos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor= thisform.meses_trans(cap_nom.mdp,i,localejercicio)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N10  Factor de recargos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N10",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor                                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N11  Recargos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N11",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                REPLACE (paso) WITH valor                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp; N12  Total Contribucion Impuestos s/ Nomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                valor=thisform.calculo("N12",(paso),,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                SKIP &amp;&amp;  N13 Enterado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                IF cap_nom.enterado == "S" THEN           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  REPLACE (paso) WITH 1 &amp;&amp;impuesto enterado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ELSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  REPLACE (paso) WITH 0 &amp;&amp;impuesto NO enterado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ENDIF </t>
+  </si>
+  <si>
+    <t>isr</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>ret iva</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>hos</t>
+  </si>
+  <si>
+    <t>Ret Suel y Asim</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Ret Prof y Arre</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Desc</t>
   </si>
 </sst>
 </file>
@@ -3386,7 +3689,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3943,6 +4246,10 @@
     <xf numFmtId="164" fontId="36" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="36" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3994,7 +4301,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Énfasis5" xfId="2" builtinId="47"/>
@@ -4412,134 +4721,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="266" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="264"/>
-      <c r="C2" s="264"/>
-      <c r="D2" s="264"/>
-      <c r="E2" s="264"/>
-      <c r="F2" s="264"/>
-      <c r="G2" s="264"/>
-      <c r="H2" s="264"/>
-      <c r="I2" s="264"/>
-      <c r="L2" s="265" t="s">
+      <c r="B2" s="266"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="266"/>
+      <c r="L2" s="267" t="s">
         <v>350</v>
       </c>
-      <c r="M2" s="265"/>
-      <c r="N2" s="265"/>
-      <c r="O2" s="265"/>
-      <c r="P2" s="265"/>
-      <c r="Q2" s="265"/>
-      <c r="R2" s="265"/>
-      <c r="S2" s="265"/>
-      <c r="T2" s="265"/>
-      <c r="W2" s="266" t="s">
+      <c r="M2" s="267"/>
+      <c r="N2" s="267"/>
+      <c r="O2" s="267"/>
+      <c r="P2" s="267"/>
+      <c r="Q2" s="267"/>
+      <c r="R2" s="267"/>
+      <c r="S2" s="267"/>
+      <c r="T2" s="267"/>
+      <c r="W2" s="268" t="s">
         <v>350</v>
       </c>
-      <c r="X2" s="266"/>
-      <c r="Y2" s="266"/>
-      <c r="Z2" s="266"/>
-      <c r="AA2" s="266"/>
-      <c r="AB2" s="266"/>
-      <c r="AC2" s="266"/>
-      <c r="AD2" s="266"/>
-      <c r="AE2" s="266"/>
-      <c r="AF2" s="266"/>
-      <c r="AK2" s="258" t="s">
+      <c r="X2" s="268"/>
+      <c r="Y2" s="268"/>
+      <c r="Z2" s="268"/>
+      <c r="AA2" s="268"/>
+      <c r="AB2" s="268"/>
+      <c r="AC2" s="268"/>
+      <c r="AD2" s="268"/>
+      <c r="AE2" s="268"/>
+      <c r="AF2" s="268"/>
+      <c r="AK2" s="260" t="s">
         <v>350</v>
       </c>
-      <c r="AL2" s="258"/>
-      <c r="AM2" s="258"/>
-      <c r="AN2" s="258"/>
-      <c r="AO2" s="258"/>
-      <c r="AP2" s="258"/>
-      <c r="AQ2" s="258"/>
-      <c r="AR2" s="258"/>
-      <c r="AS2" s="258"/>
-      <c r="AX2" s="258" t="s">
+      <c r="AL2" s="260"/>
+      <c r="AM2" s="260"/>
+      <c r="AN2" s="260"/>
+      <c r="AO2" s="260"/>
+      <c r="AP2" s="260"/>
+      <c r="AQ2" s="260"/>
+      <c r="AR2" s="260"/>
+      <c r="AS2" s="260"/>
+      <c r="AX2" s="260" t="s">
         <v>350</v>
       </c>
-      <c r="AY2" s="258"/>
-      <c r="AZ2" s="258"/>
-      <c r="BA2" s="258"/>
-      <c r="BB2" s="258"/>
-      <c r="BC2" s="258"/>
-      <c r="BD2" s="258"/>
-      <c r="BE2" s="258"/>
-      <c r="BF2" s="258"/>
+      <c r="AY2" s="260"/>
+      <c r="AZ2" s="260"/>
+      <c r="BA2" s="260"/>
+      <c r="BB2" s="260"/>
+      <c r="BC2" s="260"/>
+      <c r="BD2" s="260"/>
+      <c r="BE2" s="260"/>
+      <c r="BF2" s="260"/>
       <c r="BG2" s="197"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A4" s="269" t="s">
+      <c r="A4" s="271" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="269"/>
-      <c r="C4" s="267" t="s">
+      <c r="B4" s="271"/>
+      <c r="C4" s="269" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="262"/>
-      <c r="E4" s="262"/>
-      <c r="F4" s="262"/>
-      <c r="G4" s="262"/>
-      <c r="H4" s="262"/>
-      <c r="I4" s="263"/>
+      <c r="D4" s="264"/>
+      <c r="E4" s="264"/>
+      <c r="F4" s="264"/>
+      <c r="G4" s="264"/>
+      <c r="H4" s="264"/>
+      <c r="I4" s="265"/>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
-      <c r="L4" s="272" t="s">
+      <c r="L4" s="274" t="s">
         <v>227</v>
       </c>
-      <c r="M4" s="273"/>
+      <c r="M4" s="275"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="267" t="s">
+      <c r="O4" s="269" t="s">
         <v>285</v>
       </c>
-      <c r="P4" s="262"/>
-      <c r="Q4" s="262"/>
-      <c r="R4" s="262"/>
-      <c r="S4" s="263"/>
+      <c r="P4" s="264"/>
+      <c r="Q4" s="264"/>
+      <c r="R4" s="264"/>
+      <c r="S4" s="265"/>
       <c r="T4" s="36"/>
       <c r="U4" s="36"/>
-      <c r="W4" s="270" t="s">
+      <c r="W4" s="272" t="s">
         <v>227</v>
       </c>
-      <c r="X4" s="270"/>
+      <c r="X4" s="272"/>
       <c r="Y4" s="68"/>
-      <c r="Z4" s="271" t="s">
+      <c r="Z4" s="273" t="s">
         <v>288</v>
       </c>
-      <c r="AA4" s="271"/>
-      <c r="AB4" s="271"/>
-      <c r="AC4" s="271"/>
-      <c r="AD4" s="271"/>
-      <c r="AE4" s="271"/>
-      <c r="AF4" s="271"/>
-      <c r="AK4" s="259" t="s">
+      <c r="AA4" s="273"/>
+      <c r="AB4" s="273"/>
+      <c r="AC4" s="273"/>
+      <c r="AD4" s="273"/>
+      <c r="AE4" s="273"/>
+      <c r="AF4" s="273"/>
+      <c r="AK4" s="261" t="s">
         <v>227</v>
       </c>
-      <c r="AL4" s="260"/>
+      <c r="AL4" s="262"/>
       <c r="AM4" s="78"/>
-      <c r="AN4" s="267" t="s">
+      <c r="AN4" s="269" t="s">
         <v>364</v>
       </c>
-      <c r="AO4" s="262"/>
-      <c r="AP4" s="262"/>
-      <c r="AQ4" s="262"/>
-      <c r="AR4" s="263"/>
+      <c r="AO4" s="264"/>
+      <c r="AP4" s="264"/>
+      <c r="AQ4" s="264"/>
+      <c r="AR4" s="265"/>
       <c r="AS4" s="78"/>
       <c r="AT4" s="78"/>
-      <c r="AX4" s="259" t="s">
+      <c r="AX4" s="261" t="s">
         <v>227</v>
       </c>
-      <c r="AY4" s="260"/>
+      <c r="AY4" s="262"/>
       <c r="AZ4" s="171"/>
-      <c r="BA4" s="261" t="s">
+      <c r="BA4" s="263" t="s">
         <v>561</v>
       </c>
-      <c r="BB4" s="262"/>
-      <c r="BC4" s="262"/>
-      <c r="BD4" s="262"/>
-      <c r="BE4" s="263"/>
+      <c r="BB4" s="264"/>
+      <c r="BC4" s="264"/>
+      <c r="BD4" s="264"/>
+      <c r="BE4" s="265"/>
       <c r="BF4" s="171"/>
       <c r="BG4" s="197"/>
       <c r="BJ4" t="s">
@@ -4960,10 +5269,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="268" t="s">
+      <c r="E8" s="270" t="s">
         <v>308</v>
       </c>
-      <c r="F8" s="268"/>
+      <c r="F8" s="270"/>
       <c r="G8" s="14"/>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -9492,10 +9801,10 @@
       <c r="D52" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E52" s="268" t="s">
+      <c r="E52" s="270" t="s">
         <v>326</v>
       </c>
-      <c r="F52" s="268"/>
+      <c r="F52" s="270"/>
       <c r="G52" s="14"/>
       <c r="H52" s="5" t="s">
         <v>65</v>
@@ -9822,10 +10131,10 @@
       <c r="D56" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E56" s="268" t="s">
+      <c r="E56" s="270" t="s">
         <v>325</v>
       </c>
-      <c r="F56" s="268"/>
+      <c r="F56" s="270"/>
       <c r="G56" s="14"/>
       <c r="H56" s="5" t="s">
         <v>72</v>
@@ -10208,16 +10517,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="274" t="s">
+      <c r="A1" s="276" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="274"/>
+      <c r="B1" s="276"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
-      <c r="G1" s="274" t="s">
+      <c r="G1" s="276" t="s">
         <v>228</v>
       </c>
-      <c r="H1" s="274"/>
+      <c r="H1" s="276"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -16028,15 +16337,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>664</v>
       </c>
@@ -16047,7 +16361,27 @@
         <v>665</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" t="s">
+        <v>682</v>
+      </c>
+      <c r="G2" s="259" t="s">
+        <v>781</v>
+      </c>
+      <c r="H2" s="259" t="s">
+        <v>782</v>
+      </c>
+      <c r="I2" s="259">
+        <v>4</v>
+      </c>
+      <c r="J2" s="259">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>666</v>
       </c>
@@ -16060,8 +16394,20 @@
       <c r="D3">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="259" t="s">
+        <v>772</v>
+      </c>
+      <c r="H3" s="277" t="s">
+        <v>766</v>
+      </c>
+      <c r="I3" s="259">
+        <v>25</v>
+      </c>
+      <c r="J3" s="259">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>667</v>
       </c>
@@ -16071,11 +16417,23 @@
       <c r="C4" s="245" t="s">
         <v>681</v>
       </c>
-      <c r="F4" s="275">
+      <c r="F4" s="258">
         <v>67383.67</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="259" t="s">
+        <v>773</v>
+      </c>
+      <c r="H4" s="277" t="s">
+        <v>767</v>
+      </c>
+      <c r="I4" s="259">
+        <v>35</v>
+      </c>
+      <c r="J4" s="259">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>668</v>
       </c>
@@ -16091,8 +16449,20 @@
       <c r="F5">
         <v>1267383.67</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="259" t="s">
+        <v>774</v>
+      </c>
+      <c r="H5" s="277" t="s">
+        <v>771</v>
+      </c>
+      <c r="I5" s="259">
+        <v>35</v>
+      </c>
+      <c r="J5" s="259">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>669</v>
       </c>
@@ -16105,8 +16475,20 @@
       <c r="D6">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="259" t="s">
+        <v>778</v>
+      </c>
+      <c r="H6" s="277" t="s">
+        <v>779</v>
+      </c>
+      <c r="I6" s="259">
+        <v>35</v>
+      </c>
+      <c r="J6" s="259" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>669</v>
       </c>
@@ -16114,8 +16496,20 @@
         <v>32</v>
       </c>
       <c r="C7" s="245"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="259" t="s">
+        <v>775</v>
+      </c>
+      <c r="H7" s="277" t="s">
+        <v>768</v>
+      </c>
+      <c r="I7" s="259">
+        <v>16</v>
+      </c>
+      <c r="J7" s="259" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>670</v>
       </c>
@@ -16125,8 +16519,20 @@
       <c r="C8" s="245" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="259" t="s">
+        <v>776</v>
+      </c>
+      <c r="H8" s="277" t="s">
+        <v>769</v>
+      </c>
+      <c r="I8" s="259">
+        <v>13</v>
+      </c>
+      <c r="J8" s="259">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>670</v>
       </c>
@@ -16137,8 +16543,20 @@
       <c r="D9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="259" t="s">
+        <v>777</v>
+      </c>
+      <c r="H9" s="277" t="s">
+        <v>770</v>
+      </c>
+      <c r="I9" s="259">
+        <v>13</v>
+      </c>
+      <c r="J9" s="259">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>671</v>
       </c>
@@ -16152,7 +16570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>672</v>
       </c>
@@ -16166,7 +16584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>673</v>
       </c>
@@ -16178,6 +16596,444 @@
       </c>
       <c r="D12">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>684</v>
+      </c>
+      <c r="C14" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>684</v>
+      </c>
+      <c r="C15" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>684</v>
+      </c>
+      <c r="C16" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>687</v>
+      </c>
+      <c r="E17" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>742</v>
+      </c>
+      <c r="G73" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>747</v>
+      </c>
+      <c r="D78" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>